<commit_message>
tambah pelabuhan sapudi poi
</commit_message>
<xml_diff>
--- a/POI/Points.xlsx
+++ b/POI/Points.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28526"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Semester 7\Skripsi\Data\ArcGIS\git\aoi\POI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AD955AF-90CC-420A-AD31-C5133A7BED13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A10D0DC-1BF1-4B13-A4E0-1AA7D0BCAC79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1209" uniqueCount="561">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1218" uniqueCount="564">
   <si>
     <t>objectid</t>
   </si>
@@ -1706,6 +1706,15 @@
   </si>
   <si>
     <t xml:space="preserve">Nabire  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sapudi   </t>
+  </si>
+  <si>
+    <t>ISG</t>
+  </si>
+  <si>
+    <t>Jl. Pelabuhan No. 1 Gawam Sapudi Kab. Sumenep Madura Jawa Timur 69483</t>
   </si>
 </sst>
 </file>
@@ -2059,22 +2068,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N144"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A134" workbookViewId="0">
-      <selection activeCell="C139" sqref="C138:C139"/>
+    <sheetView tabSelected="1" topLeftCell="E131" workbookViewId="0">
+      <selection activeCell="H140" sqref="H140"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="34" customWidth="1"/>
-    <col min="8" max="8" width="45.6640625" customWidth="1"/>
+    <col min="8" max="8" width="45.7109375" customWidth="1"/>
     <col min="10" max="10" width="22" customWidth="1"/>
-    <col min="13" max="13" width="39.88671875" customWidth="1"/>
-    <col min="14" max="14" width="24.6640625" customWidth="1"/>
-    <col min="15" max="15" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="39.85546875" customWidth="1"/>
+    <col min="14" max="14" width="24.7109375" customWidth="1"/>
+    <col min="15" max="15" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2118,7 +2127,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>3</v>
       </c>
@@ -2162,7 +2171,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>11</v>
       </c>
@@ -2206,7 +2215,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>9</v>
       </c>
@@ -2250,7 +2259,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>10</v>
       </c>
@@ -2294,7 +2303,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1</v>
       </c>
@@ -2338,7 +2347,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>13</v>
       </c>
@@ -2382,7 +2391,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -2426,7 +2435,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>31</v>
       </c>
@@ -2470,7 +2479,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>21</v>
       </c>
@@ -2514,7 +2523,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>18</v>
       </c>
@@ -2558,7 +2567,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>35</v>
       </c>
@@ -2602,7 +2611,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>29</v>
       </c>
@@ -2646,7 +2655,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>19</v>
       </c>
@@ -2690,7 +2699,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>25</v>
       </c>
@@ -2734,7 +2743,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>33</v>
       </c>
@@ -2778,7 +2787,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>38</v>
       </c>
@@ -2822,7 +2831,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>32</v>
       </c>
@@ -2866,7 +2875,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>36</v>
       </c>
@@ -2910,7 +2919,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>34</v>
       </c>
@@ -2954,7 +2963,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>24</v>
       </c>
@@ -2998,7 +3007,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>48</v>
       </c>
@@ -3042,7 +3051,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>47</v>
       </c>
@@ -3086,7 +3095,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>91</v>
       </c>
@@ -3130,7 +3139,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>79</v>
       </c>
@@ -3174,7 +3183,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>82</v>
       </c>
@@ -3218,7 +3227,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>83</v>
       </c>
@@ -3262,7 +3271,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>89</v>
       </c>
@@ -3306,7 +3315,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>87</v>
       </c>
@@ -3350,7 +3359,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>88</v>
       </c>
@@ -3394,7 +3403,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>85</v>
       </c>
@@ -3438,7 +3447,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>81</v>
       </c>
@@ -3482,7 +3491,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>86</v>
       </c>
@@ -3526,7 +3535,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>103</v>
       </c>
@@ -3570,7 +3579,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>100</v>
       </c>
@@ -3614,7 +3623,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>111</v>
       </c>
@@ -3658,7 +3667,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>106</v>
       </c>
@@ -3702,7 +3711,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>96</v>
       </c>
@@ -3746,7 +3755,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>126</v>
       </c>
@@ -3790,7 +3799,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>121</v>
       </c>
@@ -3834,7 +3843,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>113</v>
       </c>
@@ -3878,7 +3887,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>114</v>
       </c>
@@ -3922,7 +3931,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>120</v>
       </c>
@@ -3966,7 +3975,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>118</v>
       </c>
@@ -4010,7 +4019,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>52</v>
       </c>
@@ -4054,7 +4063,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>54</v>
       </c>
@@ -4098,7 +4107,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>59</v>
       </c>
@@ -4142,7 +4151,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>60</v>
       </c>
@@ -4186,7 +4195,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>75</v>
       </c>
@@ -4230,7 +4239,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>146</v>
       </c>
@@ -4274,7 +4283,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>150</v>
       </c>
@@ -4318,7 +4327,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>139</v>
       </c>
@@ -4362,7 +4371,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>141</v>
       </c>
@@ -4406,7 +4415,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>143</v>
       </c>
@@ -4450,7 +4459,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>164</v>
       </c>
@@ -4494,7 +4503,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>154</v>
       </c>
@@ -4538,7 +4547,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>169</v>
       </c>
@@ -4582,7 +4591,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>171</v>
       </c>
@@ -4626,7 +4635,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>185</v>
       </c>
@@ -4670,7 +4679,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>177</v>
       </c>
@@ -4714,7 +4723,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>178</v>
       </c>
@@ -4758,7 +4767,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>192</v>
       </c>
@@ -4802,7 +4811,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>132</v>
       </c>
@@ -4846,7 +4855,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>195</v>
       </c>
@@ -4890,7 +4899,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>194</v>
       </c>
@@ -4934,7 +4943,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>211</v>
       </c>
@@ -4978,7 +4987,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>200</v>
       </c>
@@ -5022,7 +5031,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>205</v>
       </c>
@@ -5066,7 +5075,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>218</v>
       </c>
@@ -5110,7 +5119,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>219</v>
       </c>
@@ -5154,7 +5163,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>214</v>
       </c>
@@ -5198,7 +5207,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>238</v>
       </c>
@@ -5242,7 +5251,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>252</v>
       </c>
@@ -5286,7 +5295,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>236</v>
       </c>
@@ -5330,7 +5339,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>249</v>
       </c>
@@ -5374,7 +5383,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="76" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>230</v>
       </c>
@@ -5418,7 +5427,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="77" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>258</v>
       </c>
@@ -5462,7 +5471,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>269</v>
       </c>
@@ -5506,7 +5515,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="79" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>270</v>
       </c>
@@ -5550,7 +5559,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="80" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>284</v>
       </c>
@@ -5594,7 +5603,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="81" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>278</v>
       </c>
@@ -5638,7 +5647,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="82" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>279</v>
       </c>
@@ -5682,7 +5691,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="83" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>277</v>
       </c>
@@ -5726,7 +5735,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="84" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>283</v>
       </c>
@@ -5770,7 +5779,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="85" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>280</v>
       </c>
@@ -5814,7 +5823,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="86" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>281</v>
       </c>
@@ -5858,7 +5867,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="87" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>286</v>
       </c>
@@ -5902,7 +5911,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="88" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>294</v>
       </c>
@@ -5946,7 +5955,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="89" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>301</v>
       </c>
@@ -5990,7 +5999,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="90" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>304</v>
       </c>
@@ -6034,7 +6043,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="91" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>307</v>
       </c>
@@ -6078,7 +6087,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="92" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>312</v>
       </c>
@@ -6122,7 +6131,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="93" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>313</v>
       </c>
@@ -6166,7 +6175,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="94" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>308</v>
       </c>
@@ -6210,7 +6219,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="95" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>306</v>
       </c>
@@ -6254,7 +6263,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="96" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>290</v>
       </c>
@@ -6298,7 +6307,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="97" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>293</v>
       </c>
@@ -6342,7 +6351,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="98" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>317</v>
       </c>
@@ -6386,7 +6395,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="99" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>352</v>
       </c>
@@ -6430,7 +6439,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="100" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>375</v>
       </c>
@@ -6474,7 +6483,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="101" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>379</v>
       </c>
@@ -6518,7 +6527,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="102" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>373</v>
       </c>
@@ -6562,7 +6571,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="103" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>386</v>
       </c>
@@ -6606,7 +6615,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="104" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>398</v>
       </c>
@@ -6650,7 +6659,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="105" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>381</v>
       </c>
@@ -6694,7 +6703,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="106" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>431</v>
       </c>
@@ -6738,7 +6747,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="107" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>440</v>
       </c>
@@ -6782,7 +6791,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="108" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>447</v>
       </c>
@@ -6826,7 +6835,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="109" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>450</v>
       </c>
@@ -6870,7 +6879,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="110" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>400</v>
       </c>
@@ -6914,7 +6923,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="111" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>415</v>
       </c>
@@ -6958,7 +6967,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="112" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>416</v>
       </c>
@@ -7002,7 +7011,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="113" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>359</v>
       </c>
@@ -7046,7 +7055,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="114" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>358</v>
       </c>
@@ -7090,7 +7099,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="115" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>367</v>
       </c>
@@ -7134,7 +7143,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="116" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>520</v>
       </c>
@@ -7178,7 +7187,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="117" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>558</v>
       </c>
@@ -7222,7 +7231,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="118" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>525</v>
       </c>
@@ -7266,7 +7275,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="119" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>523</v>
       </c>
@@ -7310,7 +7319,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="120" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>567</v>
       </c>
@@ -7354,7 +7363,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="121" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>585</v>
       </c>
@@ -7398,7 +7407,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="122" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>506</v>
       </c>
@@ -7442,7 +7451,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="123" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>473</v>
       </c>
@@ -7486,7 +7495,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="124" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>516</v>
       </c>
@@ -7530,7 +7539,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="125" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>512</v>
       </c>
@@ -7574,7 +7583,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="126" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>496</v>
       </c>
@@ -7618,7 +7627,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="127" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>614</v>
       </c>
@@ -7662,7 +7671,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="128" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>621</v>
       </c>
@@ -7706,7 +7715,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="129" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>625</v>
       </c>
@@ -7750,7 +7759,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="130" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>628</v>
       </c>
@@ -7794,7 +7803,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="131" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>588</v>
       </c>
@@ -7838,7 +7847,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="132" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>591</v>
       </c>
@@ -7882,7 +7891,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="133" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>603</v>
       </c>
@@ -7926,7 +7935,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="134" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>611</v>
       </c>
@@ -7970,7 +7979,51 @@
         <v>23</v>
       </c>
     </row>
-    <row r="144" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A135">
+        <v>187</v>
+      </c>
+      <c r="B135">
+        <v>-7.1704711999999997</v>
+      </c>
+      <c r="C135">
+        <v>114.3265991</v>
+      </c>
+      <c r="D135" t="s">
+        <v>561</v>
+      </c>
+      <c r="E135" t="s">
+        <v>562</v>
+      </c>
+      <c r="F135" t="s">
+        <v>16</v>
+      </c>
+      <c r="G135" t="s">
+        <v>17</v>
+      </c>
+      <c r="H135" t="s">
+        <v>563</v>
+      </c>
+      <c r="I135" t="s">
+        <v>272</v>
+      </c>
+      <c r="J135" t="s">
+        <v>291</v>
+      </c>
+      <c r="K135">
+        <v>35</v>
+      </c>
+      <c r="L135">
+        <v>35.29</v>
+      </c>
+      <c r="M135" t="s">
+        <v>25</v>
+      </c>
+      <c r="N135" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="144" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C144" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
koordinat lagi lagi lagi
</commit_message>
<xml_diff>
--- a/POI/Points.xlsx
+++ b/POI/Points.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Semester 7\Skripsi\Data\ArcGIS\git\aoi\POI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A10D0DC-1BF1-4B13-A4E0-1AA7D0BCAC79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C149891-B4E3-4B22-AB86-8DD41F4CC48C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2685" yWindow="2685" windowWidth="21600" windowHeight="11235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
@@ -2068,8 +2068,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N144"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E131" workbookViewId="0">
-      <selection activeCell="H140" sqref="H140"/>
+    <sheetView tabSelected="1" topLeftCell="A81" workbookViewId="0">
+      <selection activeCell="D85" sqref="D85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4376,10 +4376,10 @@
         <v>141</v>
       </c>
       <c r="B53">
-        <v>-7.6846924000000003</v>
+        <v>-7.71508729176269</v>
       </c>
       <c r="C53">
-        <v>108.6748047</v>
+        <v>108.501925891317</v>
       </c>
       <c r="D53" t="s">
         <v>249</v>
@@ -5520,10 +5520,10 @@
         <v>270</v>
       </c>
       <c r="B79">
-        <v>1.3621825999999999</v>
+        <v>1.1983403029391</v>
       </c>
       <c r="C79">
-        <v>109.3120117</v>
+        <v>109.055470228237</v>
       </c>
       <c r="D79" t="s">
         <v>358</v>
@@ -6092,10 +6092,10 @@
         <v>312</v>
       </c>
       <c r="B92">
-        <v>0.53553119999999999</v>
+        <v>0.47340115634963897</v>
       </c>
       <c r="C92">
-        <v>117.6442007</v>
+        <v>117.601627216975</v>
       </c>
       <c r="D92" t="s">
         <v>415</v>
@@ -7500,10 +7500,10 @@
         <v>516</v>
       </c>
       <c r="B124">
-        <v>-0.69091800000000003</v>
+        <v>0.67934328869543004</v>
       </c>
       <c r="C124">
-        <v>127.45599369999999</v>
+        <v>127.45515148280499</v>
       </c>
       <c r="D124" t="s">
         <v>508</v>
@@ -7544,10 +7544,10 @@
         <v>512</v>
       </c>
       <c r="B125">
-        <v>-0.76129150000000001</v>
+        <v>0.77966800769911704</v>
       </c>
       <c r="C125">
-        <v>127.4484253</v>
+        <v>127.387653846394</v>
       </c>
       <c r="D125" t="s">
         <v>506</v>

</xml_diff>